<commit_message>
Deploying to gh-pages from @ joaobtj/rfito@9ae814414165f8a5629041e698181867a6471c89 🚀
</commit_message>
<xml_diff>
--- a/data/pareamento.xlsx
+++ b/data/pareamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/joao_tolentino_ufsc_br/Documents/GitLab/rfito/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{AD298EE7-6E9F-4233-A142-351077654E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF91C02A-34B3-4513-A15C-B54ADC68FEAD}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{AD298EE7-6E9F-4233-A142-351077654E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FD1972B-C279-47D2-908E-5AC616D54D2A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB243722-8EB7-4208-91DE-4300F6A91F87}"/>
   </bookViews>
@@ -506,28 +506,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8177B7D-E2F3-417E-8641-E3EA77CA5635}">
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:T1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" customWidth="1"/>
-    <col min="15" max="15" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.21875" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>